<commit_message>
Rest_API Code added 3
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/data.xlsx
+++ b/src/test/resources/TestData/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium\NewTechSSB_CucumberBDD_Framework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E958FD0A-25F7-415F-B28A-1363D800773D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FCEDCB-105A-4E29-8181-E32DC614CB0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18350" windowHeight="6830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>

</xml_diff>